<commit_message>
Added: structure and rendering of circuits in ckts page Added: Buy me a coffee on sidebar Added: questions for 'Name of Circuits' Added: images from 'Name of Circuits' Added: circuits table in reference.xlsx
</commit_message>
<xml_diff>
--- a/data/questions.xlsx
+++ b/data/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\ECE-Boards-Practice_st\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931FB525-A77D-46AB-AE33-2ACC74FBE5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B555196-D322-488F-AB23-09E397D6AC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F837B87B-47E8-48E8-A91E-D5D7B9A773BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F837B87B-47E8-48E8-A91E-D5D7B9A773BB}"/>
   </bookViews>
   <sheets>
     <sheet name="ECE" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="1999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3755" uniqueCount="2106">
   <si>
     <t>Subject</t>
   </si>
@@ -6272,6 +6272,327 @@
   </si>
   <si>
     <t>1 and -1</t>
+  </si>
+  <si>
+    <t>This sort of device is called a ‘heat pump’. It does not violate the Second Law of thermodynamics because all energy turns into heat energy. Thus, not breaking the first law.The work on the refrigerator adds to the heat transported from the earth both adding heat to the house. This is how some heating systems work.</t>
+  </si>
+  <si>
+    <t>ductility is the ability to change shape (drawn to wires) without breaking. It is measured by % elongation. Thus, more elongation means more ductility.</t>
+  </si>
+  <si>
+    <t>Identify the circuit shown</t>
+  </si>
+  <si>
+    <t>ckt_astableMultivibrator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_colpittsOscillator_BJT.jpg</t>
+  </si>
+  <si>
+    <t>ckt_HartleyOscillator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_integrator_1.jpg</t>
+  </si>
+  <si>
+    <t>ckt_ClappOscillator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_phaseShiftOscillator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_wienBridgeOscillator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_highPassFilter.jpg</t>
+  </si>
+  <si>
+    <t>ckt_highPassFilter_1.jpg</t>
+  </si>
+  <si>
+    <t>ckt_lowPassFilter.jpg</t>
+  </si>
+  <si>
+    <t>ckt_bandPassFilter.jpg</t>
+  </si>
+  <si>
+    <t>ckt_negEdgeTriggeredFlipFlop.jpg</t>
+  </si>
+  <si>
+    <t>ckt_differentiator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_positiveLogicANDGate.png</t>
+  </si>
+  <si>
+    <t>ckt_fullWaveRectifier.jpg</t>
+  </si>
+  <si>
+    <t>ckt_clipper.jpg</t>
+  </si>
+  <si>
+    <t>ckt_halfWaveRectifier.jpg</t>
+  </si>
+  <si>
+    <t>ckt_monostableMultivibrator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_comparator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_highIsolationANDGate.jpg</t>
+  </si>
+  <si>
+    <t>ckt_totemPole.jpg</t>
+  </si>
+  <si>
+    <t>ckt_InvertingAmplifier.jpg</t>
+  </si>
+  <si>
+    <t>ckt_antiLogAmplifier.jpg</t>
+  </si>
+  <si>
+    <t>ckt_voltageFollower.jpg</t>
+  </si>
+  <si>
+    <t>ckt_nonInvertingAmplifier.jpg</t>
+  </si>
+  <si>
+    <t>ckt_JFETShuntSwitchingCkt.jpg</t>
+  </si>
+  <si>
+    <t>ckt_doubleEndedOutput.jpg</t>
+  </si>
+  <si>
+    <t>ckt_intrumentationAmplifier.jpg</t>
+  </si>
+  <si>
+    <t>ckt_ladderNetwork.png</t>
+  </si>
+  <si>
+    <t>ckt_SeriesPassVoltageRegulator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_peakDetector.jpg</t>
+  </si>
+  <si>
+    <t>ckt_singleEndedInput.jpg</t>
+  </si>
+  <si>
+    <t>ckt_constantVoltageSrc.jpg</t>
+  </si>
+  <si>
+    <t>ckt_lowPassFilter_1.jpg</t>
+  </si>
+  <si>
+    <t>ckt_weinBridgeOscillator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_SCS.png</t>
+  </si>
+  <si>
+    <t>ckt_PositiveClamper.jpg</t>
+  </si>
+  <si>
+    <t>ckt_integrator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_logAmplifier.jpg</t>
+  </si>
+  <si>
+    <t>ckt_stepDownSwitchingRegulator.jpg</t>
+  </si>
+  <si>
+    <t>ckt_OTA.png</t>
+  </si>
+  <si>
+    <t>ckt_SCS2.png</t>
+  </si>
+  <si>
+    <t>ckt_constantCurrentSource.jpg</t>
+  </si>
+  <si>
+    <t>ckt_transresistanceAmpWithOpenCktMutResRF.jpg</t>
+  </si>
+  <si>
+    <t>ckt_clappOscillator_1.jpg</t>
+  </si>
+  <si>
+    <t>ckt_shuntVoltage.jpg</t>
+  </si>
+  <si>
+    <t>ckt_N-channel_MOSFET.png</t>
+  </si>
+  <si>
+    <t>ckt_ADC.jpg</t>
+  </si>
+  <si>
+    <t>ckt_combinationClipper.jpg</t>
+  </si>
+  <si>
+    <t>ckt_complementaryMirror.jpg</t>
+  </si>
+  <si>
+    <t>ckt_Subtractor.jpg</t>
+  </si>
+  <si>
+    <t>ckt_VaricapDiodeEqCkt.png</t>
+  </si>
+  <si>
+    <t>ckt_astableMultiVib.jpg</t>
+  </si>
+  <si>
+    <t>Astable Multivibrator</t>
+  </si>
+  <si>
+    <t>Colpitts Oscillator</t>
+  </si>
+  <si>
+    <t>Hartley Oscillator</t>
+  </si>
+  <si>
+    <t>Integrator</t>
+  </si>
+  <si>
+    <t>Clapp Oscillator</t>
+  </si>
+  <si>
+    <t>Phase Shift Oscillator</t>
+  </si>
+  <si>
+    <t>Wien Bridge Oscillator</t>
+  </si>
+  <si>
+    <t>High Pass Filter</t>
+  </si>
+  <si>
+    <t>Low Pass Filter</t>
+  </si>
+  <si>
+    <t>Band Pass Filter</t>
+  </si>
+  <si>
+    <t>negative edge triggered flip flop</t>
+  </si>
+  <si>
+    <t>Differentiator</t>
+  </si>
+  <si>
+    <t>Positive Logic AND gate</t>
+  </si>
+  <si>
+    <t>Full Wave Rectifier</t>
+  </si>
+  <si>
+    <t>Clipper</t>
+  </si>
+  <si>
+    <t>Half Wave Rectifier</t>
+  </si>
+  <si>
+    <t>Monostable multivibrator</t>
+  </si>
+  <si>
+    <t>Comparator</t>
+  </si>
+  <si>
+    <t>High Isolation AND Gate</t>
+  </si>
+  <si>
+    <t>Totem Pole</t>
+  </si>
+  <si>
+    <t>Inverting Amplifier</t>
+  </si>
+  <si>
+    <t>Anti-Log Amplifier</t>
+  </si>
+  <si>
+    <t>Voltage Follower</t>
+  </si>
+  <si>
+    <t>Non-Inverting Amplifier</t>
+  </si>
+  <si>
+    <t>JFET shunt switching circuit</t>
+  </si>
+  <si>
+    <t>Double-ended (differential) input</t>
+  </si>
+  <si>
+    <t>Instrumentation Amplifier</t>
+  </si>
+  <si>
+    <t>Ladder Network</t>
+  </si>
+  <si>
+    <t>Series-pass Voltage Regulator</t>
+  </si>
+  <si>
+    <t>Peak Detector</t>
+  </si>
+  <si>
+    <t>Single-Ended Input</t>
+  </si>
+  <si>
+    <t>Current-to-Voltage Converter</t>
+  </si>
+  <si>
+    <t>Constant Voltage Source</t>
+  </si>
+  <si>
+    <t>Wein Bridge Oscillator</t>
+  </si>
+  <si>
+    <t>SCS Terminal Names</t>
+  </si>
+  <si>
+    <t>Positive Clamper</t>
+  </si>
+  <si>
+    <t>Logarithmic Amplifier</t>
+  </si>
+  <si>
+    <t>Step-down switching regulator</t>
+  </si>
+  <si>
+    <t>OTA</t>
+  </si>
+  <si>
+    <t>SCS</t>
+  </si>
+  <si>
+    <t>Constant Current Source</t>
+  </si>
+  <si>
+    <t>Transresistance amplifier with open circuit mutual resistance RF</t>
+  </si>
+  <si>
+    <t>Shunt Voltage</t>
+  </si>
+  <si>
+    <t>N-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Combination Clipper</t>
+  </si>
+  <si>
+    <t>Complementary Mirror</t>
+  </si>
+  <si>
+    <t>Subtractor</t>
+  </si>
+  <si>
+    <t>Varicap Diode - Equivalent Circuit</t>
+  </si>
+  <si>
+    <t>ckt_currentToVoltageConverter.jpg</t>
+  </si>
+  <si>
+    <t>ckt_astableMultivibrator.png</t>
   </si>
 </sst>
 </file>
@@ -6425,8 +6746,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C046523C-39E0-436C-93D9-455D500A7748}" name="Table2" displayName="Table2" ref="A1:N439" totalsRowShown="0" dataDxfId="14">
-  <autoFilter ref="A1:N439" xr:uid="{C046523C-39E0-436C-93D9-455D500A7748}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C046523C-39E0-436C-93D9-455D500A7748}" name="Table2" displayName="Table2" ref="A1:N495" totalsRowShown="0" dataDxfId="14">
+  <autoFilter ref="A1:N495" xr:uid="{C046523C-39E0-436C-93D9-455D500A7748}"/>
   <tableColumns count="14">
     <tableColumn id="14" xr3:uid="{8C72BA36-1D4F-47F7-829C-DCB9EEAF41EC}" name="question_id" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{07904C2B-EA76-4DBD-8FF3-33191F2E4E75}" name="Subject" dataDxfId="12"/>
@@ -6744,10 +7065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35E9D52-67F4-485D-888C-11E569371290}">
-  <dimension ref="A1:N439"/>
+  <dimension ref="A1:N495"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A423" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A440" sqref="A440"/>
+    <sheetView tabSelected="1" topLeftCell="A447" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D460" sqref="D460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6755,7 +7076,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="53.42578125" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -6836,7 +7158,9 @@
       <c r="J2" s="2" t="s">
         <v>1222</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>2000</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -12079,7 +12403,7 @@
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
     </row>
-    <row r="157" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A157" s="5">
         <v>156</v>
       </c>
@@ -12108,7 +12432,9 @@
       <c r="J157" s="2" t="s">
         <v>1486</v>
       </c>
-      <c r="K157" s="1"/>
+      <c r="K157" s="1" t="s">
+        <v>1999</v>
+      </c>
       <c r="L157" s="1"/>
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
@@ -21616,6 +21942,1574 @@
       <c r="N439" s="1" t="s">
         <v>1976</v>
       </c>
+    </row>
+    <row r="440" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A440" s="5">
+        <v>439</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D440" s="2" t="s">
+        <v>2002</v>
+      </c>
+      <c r="E440" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F440" s="1" t="s">
+        <v>2055</v>
+      </c>
+      <c r="G440" s="2"/>
+      <c r="H440" s="2"/>
+      <c r="I440" s="2"/>
+      <c r="J440" s="2"/>
+      <c r="K440" s="1"/>
+      <c r="L440" s="1"/>
+      <c r="M440" s="1"/>
+      <c r="N440" s="1"/>
+    </row>
+    <row r="441" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A441" s="5">
+        <v>440</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D441" s="2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="E441" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F441" s="1" t="s">
+        <v>2056</v>
+      </c>
+      <c r="G441" s="2"/>
+      <c r="H441" s="2"/>
+      <c r="I441" s="2"/>
+      <c r="J441" s="2"/>
+      <c r="K441" s="1"/>
+      <c r="L441" s="1"/>
+      <c r="M441" s="1"/>
+      <c r="N441" s="1"/>
+    </row>
+    <row r="442" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A442" s="5">
+        <v>441</v>
+      </c>
+      <c r="B442" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D442" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="E442" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F442" s="1" t="s">
+        <v>2057</v>
+      </c>
+      <c r="G442" s="2"/>
+      <c r="H442" s="2"/>
+      <c r="I442" s="2"/>
+      <c r="J442" s="2"/>
+      <c r="K442" s="1"/>
+      <c r="L442" s="1"/>
+      <c r="M442" s="1"/>
+      <c r="N442" s="1"/>
+    </row>
+    <row r="443" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A443" s="5">
+        <v>442</v>
+      </c>
+      <c r="B443" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C443" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D443" s="2" t="s">
+        <v>2005</v>
+      </c>
+      <c r="E443" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F443" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="G443" s="2"/>
+      <c r="H443" s="2"/>
+      <c r="I443" s="2"/>
+      <c r="J443" s="2"/>
+      <c r="K443" s="1"/>
+      <c r="L443" s="1"/>
+      <c r="M443" s="1"/>
+      <c r="N443" s="1"/>
+    </row>
+    <row r="444" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A444" s="5">
+        <v>443</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D444" s="2" t="s">
+        <v>2006</v>
+      </c>
+      <c r="E444" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F444" s="1" t="s">
+        <v>2059</v>
+      </c>
+      <c r="G444" s="2"/>
+      <c r="H444" s="2"/>
+      <c r="I444" s="2"/>
+      <c r="J444" s="2"/>
+      <c r="K444" s="1"/>
+      <c r="L444" s="1"/>
+      <c r="M444" s="1"/>
+      <c r="N444" s="1"/>
+    </row>
+    <row r="445" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A445" s="5">
+        <v>444</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C445" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D445" s="2" t="s">
+        <v>2007</v>
+      </c>
+      <c r="E445" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F445" s="1" t="s">
+        <v>2060</v>
+      </c>
+      <c r="G445" s="2"/>
+      <c r="H445" s="2"/>
+      <c r="I445" s="2"/>
+      <c r="J445" s="2"/>
+      <c r="K445" s="1"/>
+      <c r="L445" s="1"/>
+      <c r="M445" s="1"/>
+      <c r="N445" s="1"/>
+    </row>
+    <row r="446" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A446" s="5">
+        <v>445</v>
+      </c>
+      <c r="B446" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C446" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D446" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="E446" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F446" s="1" t="s">
+        <v>2061</v>
+      </c>
+      <c r="G446" s="2"/>
+      <c r="H446" s="2"/>
+      <c r="I446" s="2"/>
+      <c r="J446" s="2"/>
+      <c r="K446" s="1"/>
+      <c r="L446" s="1"/>
+      <c r="M446" s="1"/>
+      <c r="N446" s="1"/>
+    </row>
+    <row r="447" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A447" s="5">
+        <v>446</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D447" s="2" t="s">
+        <v>2009</v>
+      </c>
+      <c r="E447" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F447" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="G447" s="2"/>
+      <c r="H447" s="2"/>
+      <c r="I447" s="2"/>
+      <c r="J447" s="2"/>
+      <c r="K447" s="1"/>
+      <c r="L447" s="1"/>
+      <c r="M447" s="1"/>
+      <c r="N447" s="1"/>
+    </row>
+    <row r="448" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A448" s="5">
+        <v>447</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D448" s="2" t="s">
+        <v>2010</v>
+      </c>
+      <c r="E448" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F448" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="G448" s="2"/>
+      <c r="H448" s="2"/>
+      <c r="I448" s="2"/>
+      <c r="J448" s="2"/>
+      <c r="K448" s="1"/>
+      <c r="L448" s="1"/>
+      <c r="M448" s="1"/>
+      <c r="N448" s="1"/>
+    </row>
+    <row r="449" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A449" s="5">
+        <v>448</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D449" s="2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="E449" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F449" s="1" t="s">
+        <v>2063</v>
+      </c>
+      <c r="G449" s="2"/>
+      <c r="H449" s="2"/>
+      <c r="I449" s="2"/>
+      <c r="J449" s="2"/>
+      <c r="K449" s="1"/>
+      <c r="L449" s="1"/>
+      <c r="M449" s="1"/>
+      <c r="N449" s="1"/>
+    </row>
+    <row r="450" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A450" s="5">
+        <v>449</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C450" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D450" s="2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="E450" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F450" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="G450" s="2"/>
+      <c r="H450" s="2"/>
+      <c r="I450" s="2"/>
+      <c r="J450" s="2"/>
+      <c r="K450" s="1"/>
+      <c r="L450" s="1"/>
+      <c r="M450" s="1"/>
+      <c r="N450" s="1"/>
+    </row>
+    <row r="451" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A451" s="5">
+        <v>450</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D451" s="2" t="s">
+        <v>2013</v>
+      </c>
+      <c r="E451" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F451" s="1" t="s">
+        <v>2065</v>
+      </c>
+      <c r="G451" s="2"/>
+      <c r="H451" s="2"/>
+      <c r="I451" s="2"/>
+      <c r="J451" s="2"/>
+      <c r="K451" s="1"/>
+      <c r="L451" s="1"/>
+      <c r="M451" s="1"/>
+      <c r="N451" s="1"/>
+    </row>
+    <row r="452" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A452" s="5">
+        <v>451</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D452" s="2" t="s">
+        <v>2014</v>
+      </c>
+      <c r="E452" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F452" s="1" t="s">
+        <v>2066</v>
+      </c>
+      <c r="G452" s="2"/>
+      <c r="H452" s="2"/>
+      <c r="I452" s="2"/>
+      <c r="J452" s="2"/>
+      <c r="K452" s="1"/>
+      <c r="L452" s="1"/>
+      <c r="M452" s="1"/>
+      <c r="N452" s="1"/>
+    </row>
+    <row r="453" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A453" s="5">
+        <v>452</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D453" s="2" t="s">
+        <v>2015</v>
+      </c>
+      <c r="E453" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F453" s="1" t="s">
+        <v>2067</v>
+      </c>
+      <c r="G453" s="2"/>
+      <c r="H453" s="2"/>
+      <c r="I453" s="2"/>
+      <c r="J453" s="2"/>
+      <c r="K453" s="1"/>
+      <c r="L453" s="1"/>
+      <c r="M453" s="1"/>
+      <c r="N453" s="1"/>
+    </row>
+    <row r="454" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A454" s="5">
+        <v>453</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D454" s="2" t="s">
+        <v>2016</v>
+      </c>
+      <c r="E454" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F454" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="G454" s="2"/>
+      <c r="H454" s="2"/>
+      <c r="I454" s="2"/>
+      <c r="J454" s="2"/>
+      <c r="K454" s="1"/>
+      <c r="L454" s="1"/>
+      <c r="M454" s="1"/>
+      <c r="N454" s="1"/>
+    </row>
+    <row r="455" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A455" s="5">
+        <v>454</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C455" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D455" s="2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="E455" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F455" s="1" t="s">
+        <v>2069</v>
+      </c>
+      <c r="G455" s="2"/>
+      <c r="H455" s="2"/>
+      <c r="I455" s="2"/>
+      <c r="J455" s="2"/>
+      <c r="K455" s="1"/>
+      <c r="L455" s="1"/>
+      <c r="M455" s="1"/>
+      <c r="N455" s="1"/>
+    </row>
+    <row r="456" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A456" s="5">
+        <v>455</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C456" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D456" s="2" t="s">
+        <v>2018</v>
+      </c>
+      <c r="E456" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F456" s="1" t="s">
+        <v>2070</v>
+      </c>
+      <c r="G456" s="2"/>
+      <c r="H456" s="2"/>
+      <c r="I456" s="2"/>
+      <c r="J456" s="2"/>
+      <c r="K456" s="1"/>
+      <c r="L456" s="1"/>
+      <c r="M456" s="1"/>
+      <c r="N456" s="1"/>
+    </row>
+    <row r="457" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A457" s="5">
+        <v>456</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C457" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D457" s="2" t="s">
+        <v>2019</v>
+      </c>
+      <c r="E457" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F457" s="1" t="s">
+        <v>2071</v>
+      </c>
+      <c r="G457" s="2"/>
+      <c r="H457" s="2"/>
+      <c r="I457" s="2"/>
+      <c r="J457" s="2"/>
+      <c r="K457" s="1"/>
+      <c r="L457" s="1"/>
+      <c r="M457" s="1"/>
+      <c r="N457" s="1"/>
+    </row>
+    <row r="458" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A458" s="5">
+        <v>457</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C458" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D458" s="2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="E458" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F458" s="1" t="s">
+        <v>2072</v>
+      </c>
+      <c r="G458" s="2"/>
+      <c r="H458" s="2"/>
+      <c r="I458" s="2"/>
+      <c r="J458" s="2"/>
+      <c r="K458" s="1"/>
+      <c r="L458" s="1"/>
+      <c r="M458" s="1"/>
+      <c r="N458" s="1"/>
+    </row>
+    <row r="459" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A459" s="5">
+        <v>458</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D459" s="2" t="s">
+        <v>2105</v>
+      </c>
+      <c r="E459" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F459" s="1" t="s">
+        <v>2055</v>
+      </c>
+      <c r="G459" s="2"/>
+      <c r="H459" s="2"/>
+      <c r="I459" s="2"/>
+      <c r="J459" s="2"/>
+      <c r="K459" s="1"/>
+      <c r="L459" s="1"/>
+      <c r="M459" s="1"/>
+      <c r="N459" s="1"/>
+    </row>
+    <row r="460" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A460" s="5">
+        <v>459</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D460" s="2" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E460" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F460" s="1" t="s">
+        <v>2073</v>
+      </c>
+      <c r="G460" s="2"/>
+      <c r="H460" s="2"/>
+      <c r="I460" s="2"/>
+      <c r="J460" s="2"/>
+      <c r="K460" s="1"/>
+      <c r="L460" s="1"/>
+      <c r="M460" s="1"/>
+      <c r="N460" s="1"/>
+    </row>
+    <row r="461" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A461" s="5">
+        <v>460</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D461" s="2" t="s">
+        <v>2022</v>
+      </c>
+      <c r="E461" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F461" s="1" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G461" s="2"/>
+      <c r="H461" s="2"/>
+      <c r="I461" s="2"/>
+      <c r="J461" s="2"/>
+      <c r="K461" s="1"/>
+      <c r="L461" s="1"/>
+      <c r="M461" s="1"/>
+      <c r="N461" s="1"/>
+    </row>
+    <row r="462" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A462" s="5">
+        <v>461</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C462" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D462" s="2" t="s">
+        <v>2023</v>
+      </c>
+      <c r="E462" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F462" s="1" t="s">
+        <v>2075</v>
+      </c>
+      <c r="G462" s="2"/>
+      <c r="H462" s="2"/>
+      <c r="I462" s="2"/>
+      <c r="J462" s="2"/>
+      <c r="K462" s="1"/>
+      <c r="L462" s="1"/>
+      <c r="M462" s="1"/>
+      <c r="N462" s="1"/>
+    </row>
+    <row r="463" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A463" s="5">
+        <v>462</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D463" s="2" t="s">
+        <v>2024</v>
+      </c>
+      <c r="E463" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F463" s="1" t="s">
+        <v>2076</v>
+      </c>
+      <c r="G463" s="2"/>
+      <c r="H463" s="2"/>
+      <c r="I463" s="2"/>
+      <c r="J463" s="2"/>
+      <c r="K463" s="1"/>
+      <c r="L463" s="1"/>
+      <c r="M463" s="1"/>
+      <c r="N463" s="1"/>
+    </row>
+    <row r="464" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A464" s="5">
+        <v>463</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C464" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D464" s="2" t="s">
+        <v>2025</v>
+      </c>
+      <c r="E464" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F464" s="1" t="s">
+        <v>2077</v>
+      </c>
+      <c r="G464" s="2"/>
+      <c r="H464" s="2"/>
+      <c r="I464" s="2"/>
+      <c r="J464" s="2"/>
+      <c r="K464" s="1"/>
+      <c r="L464" s="1"/>
+      <c r="M464" s="1"/>
+      <c r="N464" s="1"/>
+    </row>
+    <row r="465" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A465" s="5">
+        <v>464</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D465" s="2" t="s">
+        <v>2026</v>
+      </c>
+      <c r="E465" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F465" s="1" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G465" s="2"/>
+      <c r="H465" s="2"/>
+      <c r="I465" s="2"/>
+      <c r="J465" s="2"/>
+      <c r="K465" s="1"/>
+      <c r="L465" s="1"/>
+      <c r="M465" s="1"/>
+      <c r="N465" s="1"/>
+    </row>
+    <row r="466" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A466" s="5">
+        <v>465</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C466" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D466" s="2" t="s">
+        <v>2027</v>
+      </c>
+      <c r="E466" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F466" s="1" t="s">
+        <v>2079</v>
+      </c>
+      <c r="G466" s="2"/>
+      <c r="H466" s="2"/>
+      <c r="I466" s="2"/>
+      <c r="J466" s="2"/>
+      <c r="K466" s="1"/>
+      <c r="L466" s="1"/>
+      <c r="M466" s="1"/>
+      <c r="N466" s="1"/>
+    </row>
+    <row r="467" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A467" s="5">
+        <v>466</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C467" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D467" s="2" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E467" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F467" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="G467" s="2"/>
+      <c r="H467" s="2"/>
+      <c r="I467" s="2"/>
+      <c r="J467" s="2"/>
+      <c r="K467" s="1"/>
+      <c r="L467" s="1"/>
+      <c r="M467" s="1"/>
+      <c r="N467" s="1"/>
+    </row>
+    <row r="468" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A468" s="5">
+        <v>467</v>
+      </c>
+      <c r="B468" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C468" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D468" s="2" t="s">
+        <v>2029</v>
+      </c>
+      <c r="E468" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F468" s="1" t="s">
+        <v>2081</v>
+      </c>
+      <c r="G468" s="2"/>
+      <c r="H468" s="2"/>
+      <c r="I468" s="2"/>
+      <c r="J468" s="2"/>
+      <c r="K468" s="1"/>
+      <c r="L468" s="1"/>
+      <c r="M468" s="1"/>
+      <c r="N468" s="1"/>
+    </row>
+    <row r="469" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A469" s="5">
+        <v>468</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C469" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D469" s="2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="E469" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F469" s="1" t="s">
+        <v>2082</v>
+      </c>
+      <c r="G469" s="2"/>
+      <c r="H469" s="2"/>
+      <c r="I469" s="2"/>
+      <c r="J469" s="2"/>
+      <c r="K469" s="1"/>
+      <c r="L469" s="1"/>
+      <c r="M469" s="1"/>
+      <c r="N469" s="1"/>
+    </row>
+    <row r="470" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A470" s="5">
+        <v>469</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C470" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D470" s="2" t="s">
+        <v>2005</v>
+      </c>
+      <c r="E470" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F470" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="G470" s="2"/>
+      <c r="H470" s="2"/>
+      <c r="I470" s="2"/>
+      <c r="J470" s="2"/>
+      <c r="K470" s="1"/>
+      <c r="L470" s="1"/>
+      <c r="M470" s="1"/>
+      <c r="N470" s="1"/>
+    </row>
+    <row r="471" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A471" s="5">
+        <v>470</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C471" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D471" s="2" t="s">
+        <v>2031</v>
+      </c>
+      <c r="E471" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F471" s="1" t="s">
+        <v>2083</v>
+      </c>
+      <c r="G471" s="2"/>
+      <c r="H471" s="2"/>
+      <c r="I471" s="2"/>
+      <c r="J471" s="2"/>
+      <c r="K471" s="1"/>
+      <c r="L471" s="1"/>
+      <c r="M471" s="1"/>
+      <c r="N471" s="1"/>
+    </row>
+    <row r="472" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A472" s="5">
+        <v>471</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C472" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D472" s="2" t="s">
+        <v>2032</v>
+      </c>
+      <c r="E472" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F472" s="1" t="s">
+        <v>2084</v>
+      </c>
+      <c r="G472" s="2"/>
+      <c r="H472" s="2"/>
+      <c r="I472" s="2"/>
+      <c r="J472" s="2"/>
+      <c r="K472" s="1"/>
+      <c r="L472" s="1"/>
+      <c r="M472" s="1"/>
+      <c r="N472" s="1"/>
+    </row>
+    <row r="473" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A473" s="5">
+        <v>472</v>
+      </c>
+      <c r="B473" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C473" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D473" s="2" t="s">
+        <v>2033</v>
+      </c>
+      <c r="E473" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F473" s="1" t="s">
+        <v>2085</v>
+      </c>
+      <c r="G473" s="2"/>
+      <c r="H473" s="2"/>
+      <c r="I473" s="2"/>
+      <c r="J473" s="2"/>
+      <c r="K473" s="1"/>
+      <c r="L473" s="1"/>
+      <c r="M473" s="1"/>
+      <c r="N473" s="1"/>
+    </row>
+    <row r="474" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A474" s="5">
+        <v>473</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C474" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D474" s="2" t="s">
+        <v>2104</v>
+      </c>
+      <c r="E474" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F474" s="1" t="s">
+        <v>2086</v>
+      </c>
+      <c r="G474" s="2"/>
+      <c r="H474" s="2"/>
+      <c r="I474" s="2"/>
+      <c r="J474" s="2"/>
+      <c r="K474" s="1"/>
+      <c r="L474" s="1"/>
+      <c r="M474" s="1"/>
+      <c r="N474" s="1"/>
+    </row>
+    <row r="475" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A475" s="5">
+        <v>474</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C475" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D475" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="E475" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F475" s="1" t="s">
+        <v>2087</v>
+      </c>
+      <c r="G475" s="2"/>
+      <c r="H475" s="2"/>
+      <c r="I475" s="2"/>
+      <c r="J475" s="2"/>
+      <c r="K475" s="1"/>
+      <c r="L475" s="1"/>
+      <c r="M475" s="1"/>
+      <c r="N475" s="1"/>
+    </row>
+    <row r="476" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A476" s="5">
+        <v>475</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C476" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D476" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="E476" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F476" s="1" t="s">
+        <v>2063</v>
+      </c>
+      <c r="G476" s="2"/>
+      <c r="H476" s="2"/>
+      <c r="I476" s="2"/>
+      <c r="J476" s="2"/>
+      <c r="K476" s="1"/>
+      <c r="L476" s="1"/>
+      <c r="M476" s="1"/>
+      <c r="N476" s="1"/>
+    </row>
+    <row r="477" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A477" s="5">
+        <v>476</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C477" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D477" s="2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="E477" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F477" s="1" t="s">
+        <v>2088</v>
+      </c>
+      <c r="G477" s="2"/>
+      <c r="H477" s="2"/>
+      <c r="I477" s="2"/>
+      <c r="J477" s="2"/>
+      <c r="K477" s="1"/>
+      <c r="L477" s="1"/>
+      <c r="M477" s="1"/>
+      <c r="N477" s="1"/>
+    </row>
+    <row r="478" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A478" s="5">
+        <v>477</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C478" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D478" s="2" t="s">
+        <v>2037</v>
+      </c>
+      <c r="E478" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F478" s="1" t="s">
+        <v>2089</v>
+      </c>
+      <c r="G478" s="2"/>
+      <c r="H478" s="2"/>
+      <c r="I478" s="2"/>
+      <c r="J478" s="2"/>
+      <c r="K478" s="1"/>
+      <c r="L478" s="1"/>
+      <c r="M478" s="1"/>
+      <c r="N478" s="1"/>
+    </row>
+    <row r="479" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A479" s="5">
+        <v>478</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C479" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D479" s="2" t="s">
+        <v>2038</v>
+      </c>
+      <c r="E479" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F479" s="1" t="s">
+        <v>2090</v>
+      </c>
+      <c r="G479" s="2"/>
+      <c r="H479" s="2"/>
+      <c r="I479" s="2"/>
+      <c r="J479" s="2"/>
+      <c r="K479" s="1"/>
+      <c r="L479" s="1"/>
+      <c r="M479" s="1"/>
+      <c r="N479" s="1"/>
+    </row>
+    <row r="480" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A480" s="5">
+        <v>479</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C480" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D480" s="2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="E480" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F480" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="G480" s="2"/>
+      <c r="H480" s="2"/>
+      <c r="I480" s="2"/>
+      <c r="J480" s="2"/>
+      <c r="K480" s="1"/>
+      <c r="L480" s="1"/>
+      <c r="M480" s="1"/>
+      <c r="N480" s="1"/>
+    </row>
+    <row r="481" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A481" s="5">
+        <v>480</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C481" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D481" s="2" t="s">
+        <v>2040</v>
+      </c>
+      <c r="E481" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F481" s="1" t="s">
+        <v>2091</v>
+      </c>
+      <c r="G481" s="2"/>
+      <c r="H481" s="2"/>
+      <c r="I481" s="2"/>
+      <c r="J481" s="2"/>
+      <c r="K481" s="1"/>
+      <c r="L481" s="1"/>
+      <c r="M481" s="1"/>
+      <c r="N481" s="1"/>
+    </row>
+    <row r="482" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A482" s="5">
+        <v>481</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C482" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D482" s="2" t="s">
+        <v>2041</v>
+      </c>
+      <c r="E482" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F482" s="1" t="s">
+        <v>2092</v>
+      </c>
+      <c r="G482" s="2"/>
+      <c r="H482" s="2"/>
+      <c r="I482" s="2"/>
+      <c r="J482" s="2"/>
+      <c r="K482" s="1"/>
+      <c r="L482" s="1"/>
+      <c r="M482" s="1"/>
+      <c r="N482" s="1"/>
+    </row>
+    <row r="483" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A483" s="5">
+        <v>482</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C483" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D483" s="2" t="s">
+        <v>2042</v>
+      </c>
+      <c r="E483" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F483" s="1" t="s">
+        <v>2093</v>
+      </c>
+      <c r="G483" s="2"/>
+      <c r="H483" s="2"/>
+      <c r="I483" s="2"/>
+      <c r="J483" s="2"/>
+      <c r="K483" s="1"/>
+      <c r="L483" s="1"/>
+      <c r="M483" s="1"/>
+      <c r="N483" s="1"/>
+    </row>
+    <row r="484" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A484" s="5">
+        <v>483</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C484" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D484" s="2" t="s">
+        <v>2043</v>
+      </c>
+      <c r="E484" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F484" s="1" t="s">
+        <v>2094</v>
+      </c>
+      <c r="G484" s="2"/>
+      <c r="H484" s="2"/>
+      <c r="I484" s="2"/>
+      <c r="J484" s="2"/>
+      <c r="K484" s="1"/>
+      <c r="L484" s="1"/>
+      <c r="M484" s="1"/>
+      <c r="N484" s="1"/>
+    </row>
+    <row r="485" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A485" s="5">
+        <v>484</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C485" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D485" s="2" t="s">
+        <v>2044</v>
+      </c>
+      <c r="E485" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F485" s="1" t="s">
+        <v>2095</v>
+      </c>
+      <c r="G485" s="2"/>
+      <c r="H485" s="2"/>
+      <c r="I485" s="2"/>
+      <c r="J485" s="2"/>
+      <c r="K485" s="1"/>
+      <c r="L485" s="1"/>
+      <c r="M485" s="1"/>
+      <c r="N485" s="1"/>
+    </row>
+    <row r="486" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A486" s="5">
+        <v>485</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C486" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D486" s="2" t="s">
+        <v>2045</v>
+      </c>
+      <c r="E486" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F486" s="1" t="s">
+        <v>2096</v>
+      </c>
+      <c r="G486" s="2"/>
+      <c r="H486" s="2"/>
+      <c r="I486" s="2"/>
+      <c r="J486" s="2"/>
+      <c r="K486" s="1"/>
+      <c r="L486" s="1"/>
+      <c r="M486" s="1"/>
+      <c r="N486" s="1"/>
+    </row>
+    <row r="487" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A487" s="5">
+        <v>486</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C487" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D487" s="2" t="s">
+        <v>2046</v>
+      </c>
+      <c r="E487" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F487" s="1" t="s">
+        <v>2059</v>
+      </c>
+      <c r="G487" s="2"/>
+      <c r="H487" s="2"/>
+      <c r="I487" s="2"/>
+      <c r="J487" s="2"/>
+      <c r="K487" s="1"/>
+      <c r="L487" s="1"/>
+      <c r="M487" s="1"/>
+      <c r="N487" s="1"/>
+    </row>
+    <row r="488" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A488" s="5">
+        <v>487</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C488" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D488" s="2" t="s">
+        <v>2047</v>
+      </c>
+      <c r="E488" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F488" s="1" t="s">
+        <v>2097</v>
+      </c>
+      <c r="G488" s="2"/>
+      <c r="H488" s="2"/>
+      <c r="I488" s="2"/>
+      <c r="J488" s="2"/>
+      <c r="K488" s="1"/>
+      <c r="L488" s="1"/>
+      <c r="M488" s="1"/>
+      <c r="N488" s="1"/>
+    </row>
+    <row r="489" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A489" s="5">
+        <v>488</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C489" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D489" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E489" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F489" s="1" t="s">
+        <v>2098</v>
+      </c>
+      <c r="G489" s="2"/>
+      <c r="H489" s="2"/>
+      <c r="I489" s="2"/>
+      <c r="J489" s="2"/>
+      <c r="K489" s="1"/>
+      <c r="L489" s="1"/>
+      <c r="M489" s="1"/>
+      <c r="N489" s="1"/>
+    </row>
+    <row r="490" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A490" s="5">
+        <v>489</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C490" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D490" s="2" t="s">
+        <v>2049</v>
+      </c>
+      <c r="E490" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F490" s="1" t="s">
+        <v>2099</v>
+      </c>
+      <c r="G490" s="2"/>
+      <c r="H490" s="2"/>
+      <c r="I490" s="2"/>
+      <c r="J490" s="2"/>
+      <c r="K490" s="1"/>
+      <c r="L490" s="1"/>
+      <c r="M490" s="1"/>
+      <c r="N490" s="1"/>
+    </row>
+    <row r="491" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A491" s="5">
+        <v>490</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C491" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D491" s="2" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E491" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F491" s="1" t="s">
+        <v>2100</v>
+      </c>
+      <c r="G491" s="2"/>
+      <c r="H491" s="2"/>
+      <c r="I491" s="2"/>
+      <c r="J491" s="2"/>
+      <c r="K491" s="1"/>
+      <c r="L491" s="1"/>
+      <c r="M491" s="1"/>
+      <c r="N491" s="1"/>
+    </row>
+    <row r="492" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A492" s="5">
+        <v>491</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C492" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D492" s="2" t="s">
+        <v>2051</v>
+      </c>
+      <c r="E492" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F492" s="1" t="s">
+        <v>2101</v>
+      </c>
+      <c r="G492" s="2"/>
+      <c r="H492" s="2"/>
+      <c r="I492" s="2"/>
+      <c r="J492" s="2"/>
+      <c r="K492" s="1"/>
+      <c r="L492" s="1"/>
+      <c r="M492" s="1"/>
+      <c r="N492" s="1"/>
+    </row>
+    <row r="493" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A493" s="5">
+        <v>492</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C493" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D493" s="2" t="s">
+        <v>2052</v>
+      </c>
+      <c r="E493" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F493" s="1" t="s">
+        <v>2102</v>
+      </c>
+      <c r="G493" s="2"/>
+      <c r="H493" s="2"/>
+      <c r="I493" s="2"/>
+      <c r="J493" s="2"/>
+      <c r="K493" s="1"/>
+      <c r="L493" s="1"/>
+      <c r="M493" s="1"/>
+      <c r="N493" s="1"/>
+    </row>
+    <row r="494" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A494" s="5">
+        <v>493</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C494" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D494" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="E494" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F494" s="1" t="s">
+        <v>2103</v>
+      </c>
+      <c r="G494" s="2"/>
+      <c r="H494" s="2"/>
+      <c r="I494" s="2"/>
+      <c r="J494" s="2"/>
+      <c r="K494" s="1"/>
+      <c r="L494" s="1"/>
+      <c r="M494" s="1"/>
+      <c r="N494" s="1"/>
+    </row>
+    <row r="495" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A495" s="5">
+        <v>494</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C495" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D495" s="2" t="s">
+        <v>2054</v>
+      </c>
+      <c r="E495" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F495" s="1" t="s">
+        <v>2055</v>
+      </c>
+      <c r="G495" s="2"/>
+      <c r="H495" s="2"/>
+      <c r="I495" s="2"/>
+      <c r="J495" s="2"/>
+      <c r="K495" s="1"/>
+      <c r="L495" s="1"/>
+      <c r="M495" s="1"/>
+      <c r="N495" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>